<commit_message>
Payment extensibility with factory
</commit_message>
<xml_diff>
--- a/FOMS/data/order_list.xlsx
+++ b/FOMS/data/order_list.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>10.3</t>
+  </si>
+  <si>
+    <t>6.9</t>
+  </si>
+  <si>
+    <t>PayPal</t>
   </si>
 </sst>
 </file>
@@ -539,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D9B652-E5C7-AB48-B074-FB8F261F35A4}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
@@ -892,6 +898,32 @@
         <v>8</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>